<commit_message>
All basic tarrains, L01r03 completation,
</commit_message>
<xml_diff>
--- a/Stavy jednotlivých kol.xlsx
+++ b/Stavy jednotlivých kol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="23">
   <si>
     <t>LEVEL 1</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Rnd 04</t>
   </si>
   <si>
-    <t>Enemies</t>
-  </si>
-  <si>
     <t>Coins</t>
   </si>
   <si>
@@ -63,9 +60,6 @@
     <t>Dialogs</t>
   </si>
   <si>
-    <t>Teren ok, collider will be done</t>
-  </si>
-  <si>
     <t>Basic terrain</t>
   </si>
   <si>
@@ -73,6 +67,24 @@
   </si>
   <si>
     <t>doplnit</t>
+  </si>
+  <si>
+    <t>Camera triggers</t>
+  </si>
+  <si>
+    <t>Undeads</t>
+  </si>
+  <si>
+    <t>Jen příprava, chybí texty</t>
+  </si>
+  <si>
+    <t>Restart floor</t>
+  </si>
+  <si>
+    <t>dořešit, funguje divně</t>
+  </si>
+  <si>
+    <t>Change scene</t>
   </si>
 </sst>
 </file>
@@ -123,7 +135,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,12 +156,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -157,6 +163,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -369,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -382,15 +400,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -687,22 +706,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="23.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.42578125" customWidth="1"/>
     <col min="2" max="4" width="11.28515625" customWidth="1"/>
-    <col min="5" max="5" width="29.42578125" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.42578125" customWidth="1"/>
     <col min="7" max="10" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="15.75" thickBot="1">
       <c r="A1" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" s="12"/>
       <c r="C1" s="12"/>
@@ -712,7 +731,7 @@
     </row>
     <row r="2" spans="1:10" ht="18.75">
       <c r="A2" s="13" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>0</v>
@@ -726,8 +745,8 @@
       <c r="E2" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="18" t="s">
-        <v>17</v>
+      <c r="F2" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>0</v>
@@ -747,31 +766,31 @@
         <v>4</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E3" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="18" t="s">
         <v>4</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -779,31 +798,31 @@
         <v>5</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="18" t="s">
         <v>5</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -811,31 +830,31 @@
         <v>6</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>18</v>
+      <c r="G5" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1">
@@ -843,36 +862,36 @@
         <v>7</v>
       </c>
       <c r="B6" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="19" t="s">
         <v>7</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="J6" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.100000000000001" customHeight="1">
-      <c r="A7" s="18" t="s">
-        <v>10</v>
+      <c r="A7" s="17" t="s">
+        <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>0</v>
@@ -886,78 +905,153 @@
       <c r="E7" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="F7" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J7" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="19" t="s">
+      <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="19" t="s">
+      <c r="A10" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>18</v>
+      <c r="B10" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="18.75">
       <c r="A12" s="13" t="s">
-        <v>8</v>
+        <v>18</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>0</v>
@@ -971,78 +1065,153 @@
       <c r="E12" s="7" t="s">
         <v>3</v>
       </c>
+      <c r="F12" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J12" s="7" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="19" t="s">
+      <c r="A13" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>18</v>
+      <c r="B13" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="19" t="s">
+      <c r="A14" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>18</v>
+      <c r="B14" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="19" t="s">
+      <c r="A15" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>18</v>
+      <c r="B15" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A16" s="20" t="s">
+      <c r="A16" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="18.75">
+        <v>16</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="18.75">
       <c r="A17" s="13" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>0</v>
@@ -1056,78 +1225,153 @@
       <c r="E17" s="7" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="A18" s="19" t="s">
+      <c r="F17" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
+      <c r="A18" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>18</v>
+      <c r="B18" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
+      <c r="A19" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>18</v>
+      <c r="B19" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="A20" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>18</v>
+      <c r="B20" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A21" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>6</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A21" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="18.75">
+        <v>16</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="18.75">
       <c r="A22" s="13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>0</v>
@@ -1142,77 +1386,77 @@
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
-      <c r="A23" s="19" t="s">
+    <row r="23" spans="1:10">
+      <c r="A23" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>18</v>
+      <c r="B23" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5">
-      <c r="A24" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10">
+      <c r="A24" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>18</v>
+      <c r="B24" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10">
+      <c r="A25" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>18</v>
+      <c r="B25" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A26" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A26" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="18.75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="18.75">
       <c r="A27" s="13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>0</v>
@@ -1227,72 +1471,72 @@
         <v>3</v>
       </c>
     </row>
-    <row r="28" spans="1:5">
-      <c r="A28" s="19" t="s">
+    <row r="28" spans="1:10">
+      <c r="A28" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="2" t="s">
-        <v>18</v>
+      <c r="B28" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5">
-      <c r="A29" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10">
+      <c r="A29" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="2" t="s">
-        <v>18</v>
+      <c r="B29" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>18</v>
+      <c r="B30" s="20" t="s">
+        <v>19</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A31" s="20" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A31" s="19" t="s">
         <v>7</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
L01r04 terrain completion(no fighting), view table
</commit_message>
<xml_diff>
--- a/Stavy jednotlivých kol.xlsx
+++ b/Stavy jednotlivých kol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="25">
   <si>
     <t>LEVEL 1</t>
   </si>
@@ -85,6 +85,12 @@
   </si>
   <si>
     <t>Change scene</t>
+  </si>
+  <si>
+    <t>není třeba</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -135,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -178,6 +184,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -387,7 +399,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -410,6 +422,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -707,7 +720,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -876,8 +889,8 @@
       <c r="F6" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G6" s="4" t="s">
-        <v>16</v>
+      <c r="G6" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>16</v>
@@ -925,8 +938,8 @@
       <c r="A8" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>16</v>
+      <c r="B8" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>16</v>
@@ -957,8 +970,8 @@
       <c r="A9" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>16</v>
+      <c r="B9" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>16</v>
@@ -1021,8 +1034,8 @@
       <c r="A11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>16</v>
+      <c r="B11" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>16</v>
@@ -1036,8 +1049,8 @@
       <c r="F11" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>16</v>
+      <c r="G11" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>16</v>
@@ -1196,11 +1209,11 @@
       <c r="F16" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="4" t="s">
-        <v>16</v>
+      <c r="G16" s="22" t="s">
+        <v>23</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I16" s="4" t="s">
         <v>16</v>
@@ -1260,8 +1273,8 @@
       <c r="F18" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>16</v>
+      <c r="G18" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="H18" s="2" t="s">
         <v>16</v>
@@ -1292,8 +1305,8 @@
       <c r="F19" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>16</v>
+      <c r="G19" s="10" t="s">
+        <v>10</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>16</v>
@@ -1341,8 +1354,8 @@
       <c r="A21" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>16</v>
+      <c r="B21" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>16</v>
@@ -1356,8 +1369,8 @@
       <c r="F21" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="4" t="s">
-        <v>16</v>
+      <c r="G21" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Beginning of wraith fight
</commit_message>
<xml_diff>
--- a/Stavy jednotlivých kol.xlsx
+++ b/Stavy jednotlivých kol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="27">
   <si>
     <t>LEVEL 1</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>nefunguje</t>
+  </si>
+  <si>
+    <t>L01R03 OPRAVIT HOD OŠTĚPU PŘI POHYBU, JEN PŘI ZASTAVENÍ</t>
   </si>
 </sst>
 </file>
@@ -413,7 +416,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -439,6 +442,7 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -736,7 +740,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1505,8 +1509,8 @@
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>15</v>
+      <c r="C25" s="25" t="s">
+        <v>26</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Dialogs for 3rd RND and some changes of code
Musel jsem změnit některé funkcionality v dialozích a v enemybehaviour
(charon umre a vyvola se posledni dialog)
</commit_message>
<xml_diff>
--- a/Stavy jednotlivých kol.xlsx
+++ b/Stavy jednotlivých kol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="25">
   <si>
     <t>LEVEL 1</t>
   </si>
@@ -72,9 +72,6 @@
     <t>Undeads</t>
   </si>
   <si>
-    <t>Jen příprava, chybí texty</t>
-  </si>
-  <si>
     <t>Restart floor</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
   </si>
   <si>
     <t>nefunguje</t>
-  </si>
-  <si>
-    <t>L01R03 OPRAVIT HOD OŠTĚPU PŘI POHYBU, JEN PŘI ZASTAVENÍ</t>
   </si>
 </sst>
 </file>
@@ -147,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -169,12 +163,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -416,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -434,15 +422,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -740,7 +726,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -753,18 +739,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10" ht="18.75">
       <c r="A2" s="11" t="s">
@@ -1103,7 +1089,7 @@
         <v>3</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>0</v>
@@ -1137,8 +1123,8 @@
       <c r="F13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="20" t="s">
-        <v>21</v>
+      <c r="G13" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>15</v>
@@ -1169,8 +1155,8 @@
       <c r="F14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="20" t="s">
-        <v>21</v>
+      <c r="G14" s="19" t="s">
+        <v>20</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>15</v>
@@ -1233,11 +1219,11 @@
       <c r="F16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>21</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="I16" s="3" t="s">
         <v>15</v>
@@ -1263,7 +1249,7 @@
         <v>3</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>0</v>
@@ -1408,7 +1394,7 @@
     </row>
     <row r="22" spans="1:10" ht="18.75">
       <c r="A22" s="11" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>0</v>
@@ -1423,7 +1409,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>0</v>
@@ -1509,8 +1495,8 @@
       <c r="B25" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="25" t="s">
-        <v>26</v>
+      <c r="C25" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="D25" s="1" t="s">
         <v>15</v>
@@ -1521,8 +1507,8 @@
       <c r="F25" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="18" t="s">
-        <v>25</v>
+      <c r="G25" s="17" t="s">
+        <v>24</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>15</v>
@@ -1553,8 +1539,8 @@
       <c r="F26" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="21" t="s">
-        <v>25</v>
+      <c r="G26" s="20" t="s">
+        <v>24</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>15</v>
@@ -1587,9 +1573,7 @@
       <c r="A28" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="B28" s="9"/>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
@@ -1604,9 +1588,7 @@
       <c r="A29" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>10</v>
-      </c>
+      <c r="B29" s="9"/>
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
@@ -1621,8 +1603,8 @@
       <c r="A30" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="17" t="s">
-        <v>18</v>
+      <c r="B30" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>15</v>
@@ -1638,9 +1620,7 @@
       <c r="A31" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>15</v>
-      </c>
+      <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
LVL01RND04 dialogs and small change in trap
</commit_message>
<xml_diff>
--- a/Stavy jednotlivých kol.xlsx
+++ b/Stavy jednotlivých kol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="25">
   <si>
     <t>LEVEL 1</t>
   </si>
@@ -404,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
@@ -422,7 +422,6 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
@@ -726,7 +725,7 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -739,18 +738,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="17.25" customHeight="1" thickBot="1">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
     </row>
     <row r="2" spans="1:10" ht="18.75">
       <c r="A2" s="11" t="s">
@@ -1123,7 +1122,7 @@
       <c r="F13" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G13" s="19" t="s">
+      <c r="G13" s="18" t="s">
         <v>20</v>
       </c>
       <c r="H13" s="1" t="s">
@@ -1155,7 +1154,7 @@
       <c r="F14" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="G14" s="19" t="s">
+      <c r="G14" s="18" t="s">
         <v>20</v>
       </c>
       <c r="H14" s="1" t="s">
@@ -1219,7 +1218,7 @@
       <c r="F16" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="17" t="s">
         <v>20</v>
       </c>
       <c r="H16" s="3" t="s">
@@ -1507,8 +1506,8 @@
       <c r="F25" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="G25" s="17" t="s">
-        <v>24</v>
+      <c r="G25" s="9" t="s">
+        <v>10</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>15</v>
@@ -1539,7 +1538,7 @@
       <c r="F26" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="20" t="s">
+      <c r="G26" s="19" t="s">
         <v>24</v>
       </c>
       <c r="H26" s="3" t="s">
@@ -1573,7 +1572,9 @@
       <c r="A28" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="B28" s="9"/>
+      <c r="B28" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="C28" s="1" t="s">
         <v>15</v>
       </c>
@@ -1588,7 +1589,9 @@
       <c r="A29" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="B29" s="9"/>
+      <c r="B29" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
@@ -1620,7 +1623,9 @@
       <c r="A31" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="9" t="s">
+        <v>10</v>
+      </c>
       <c r="C31" s="3" t="s">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
lvl02rnd02 part of basic stuff
</commit_message>
<xml_diff>
--- a/Stavy jednotlivých kol.xlsx
+++ b/Stavy jednotlivých kol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="28">
   <si>
     <t>LEVEL 1</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>DOPLNIT POCITADLO LEVELU</t>
+  </si>
+  <si>
+    <t>POLOVINA</t>
   </si>
 </sst>
 </file>
@@ -733,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1067,8 +1070,8 @@
       <c r="B9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
+      <c r="C9" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D9" s="19" t="s">
         <v>15</v>
@@ -1387,8 +1390,8 @@
       <c r="B19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>15</v>
+      <c r="C19" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D19" s="19" t="s">
         <v>15</v>
@@ -1563,7 +1566,7 @@
         <v>10</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="I24" s="19" t="s">
         <v>15</v>
@@ -1678,7 +1681,7 @@
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
All terrains attached soma basic stuff done
</commit_message>
<xml_diff>
--- a/Stavy jednotlivých kol.xlsx
+++ b/Stavy jednotlivých kol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="26">
   <si>
     <t>LEVEL 1</t>
   </si>
@@ -91,12 +91,6 @@
   </si>
   <si>
     <t>Black Quads around terrain</t>
-  </si>
-  <si>
-    <t>PŘIPRAVENO</t>
-  </si>
-  <si>
-    <t>DOPLNIT POCITADLO LEVELU</t>
   </si>
   <si>
     <t>POLOVINA</t>
@@ -736,8 +730,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C29" sqref="C29"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5:H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -833,8 +827,8 @@
       <c r="G3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>15</v>
+      <c r="H3" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I3" s="19" t="s">
         <v>15</v>
@@ -848,8 +842,8 @@
       <c r="L3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>25</v>
+      <c r="M3" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="N3" s="19" t="s">
         <v>15</v>
@@ -880,8 +874,8 @@
       <c r="G4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="1" t="s">
-        <v>15</v>
+      <c r="H4" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I4" s="19" t="s">
         <v>15</v>
@@ -895,8 +889,8 @@
       <c r="L4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>15</v>
+      <c r="M4" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="N4" s="19" t="s">
         <v>15</v>
@@ -927,8 +921,8 @@
       <c r="G5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H5" s="1" t="s">
-        <v>15</v>
+      <c r="H5" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I5" s="19" t="s">
         <v>15</v>
@@ -942,8 +936,8 @@
       <c r="L5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>15</v>
+      <c r="M5" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="N5" s="19" t="s">
         <v>15</v>
@@ -974,8 +968,8 @@
       <c r="G6" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>15</v>
+      <c r="H6" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I6" s="21" t="s">
         <v>15</v>
@@ -989,8 +983,8 @@
       <c r="L6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>15</v>
+      <c r="M6" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="N6" s="21" t="s">
         <v>15</v>
@@ -1085,8 +1079,8 @@
       <c r="G9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>15</v>
+      <c r="H9" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I9" s="19" t="s">
         <v>15</v>
@@ -1213,8 +1207,8 @@
       <c r="G13" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H13" s="1" t="s">
-        <v>25</v>
+      <c r="H13" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I13" s="19" t="s">
         <v>15</v>
@@ -1245,8 +1239,8 @@
       <c r="G14" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="1" t="s">
-        <v>15</v>
+      <c r="H14" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I14" s="19" t="s">
         <v>15</v>
@@ -1277,8 +1271,8 @@
       <c r="G15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H15" s="1" t="s">
-        <v>15</v>
+      <c r="H15" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I15" s="19" t="s">
         <v>15</v>
@@ -1309,8 +1303,8 @@
       <c r="G16" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="1" t="s">
-        <v>15</v>
+      <c r="H16" s="12" t="s">
+        <v>20</v>
       </c>
       <c r="I16" s="21" t="s">
         <v>15</v>
@@ -1405,8 +1399,8 @@
       <c r="G19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H19" s="1" t="s">
-        <v>15</v>
+      <c r="H19" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I19" s="19" t="s">
         <v>15</v>
@@ -1533,8 +1527,8 @@
       <c r="G23" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H23" s="1" t="s">
-        <v>26</v>
+      <c r="H23" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I23" s="19" t="s">
         <v>15</v>
@@ -1565,8 +1559,8 @@
       <c r="G24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H24" s="1" t="s">
-        <v>26</v>
+      <c r="H24" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I24" s="19" t="s">
         <v>15</v>
@@ -1681,7 +1675,7 @@
         <v>10</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Basic stuff till RND03
</commit_message>
<xml_diff>
--- a/Stavy jednotlivých kol.xlsx
+++ b/Stavy jednotlivých kol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="26">
   <si>
     <t>LEVEL 1</t>
   </si>
@@ -93,7 +93,7 @@
     <t>Black Quads around terrain</t>
   </si>
   <si>
-    <t>POLOVINA</t>
+    <t>CHAMP</t>
   </si>
 </sst>
 </file>
@@ -144,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -187,6 +187,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="16">
     <border>
@@ -407,7 +413,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
@@ -434,6 +440,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="normální" xfId="0" builtinId="0"/>
@@ -731,7 +739,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5:H6"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1111,8 +1119,8 @@
       <c r="G10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H10" s="1" t="s">
-        <v>15</v>
+      <c r="H10" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I10" s="19" t="s">
         <v>15</v>
@@ -1224,8 +1232,8 @@
       <c r="B14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="1" t="s">
-        <v>15</v>
+      <c r="C14" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D14" s="19" t="s">
         <v>15</v>
@@ -1416,8 +1424,8 @@
       <c r="B20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>15</v>
+      <c r="C20" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D20" s="19" t="s">
         <v>15</v>
@@ -1431,8 +1439,8 @@
       <c r="G20" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H20" s="1" t="s">
-        <v>15</v>
+      <c r="H20" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I20" s="19" t="s">
         <v>15</v>
@@ -1544,8 +1552,8 @@
       <c r="B24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>15</v>
+      <c r="C24" s="26" t="s">
+        <v>25</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>15</v>
@@ -1576,8 +1584,9 @@
       <c r="B25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C25" s="1" t="s">
-        <v>15</v>
+      <c r="C25" s="27" t="str">
+        <f>C15</f>
+        <v>doplnit</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>15</v>
@@ -1591,8 +1600,8 @@
       <c r="G25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H25" s="1" t="s">
-        <v>15</v>
+      <c r="H25" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="I25" s="19" t="s">
         <v>15</v>
@@ -1674,8 +1683,8 @@
       <c r="B29" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C29" s="1" t="s">
-        <v>25</v>
+      <c r="C29" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D29" s="19" t="s">
         <v>15</v>
@@ -1691,8 +1700,8 @@
       <c r="B30" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C30" s="1" t="s">
-        <v>15</v>
+      <c r="C30" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D30" s="19" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
Wraiths in RND03 - problematicke
</commit_message>
<xml_diff>
--- a/Stavy jednotlivých kol.xlsx
+++ b/Stavy jednotlivých kol.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="26">
   <si>
     <t>LEVEL 1</t>
   </si>
@@ -739,7 +739,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1104,8 +1104,8 @@
       <c r="B10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
+      <c r="C10" s="6" t="s">
+        <v>10</v>
       </c>
       <c r="D10" s="19" t="s">
         <v>15</v>
@@ -1264,8 +1264,9 @@
       <c r="B15" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C15" s="1" t="s">
-        <v>15</v>
+      <c r="C15" s="27" t="str">
+        <f>C5</f>
+        <v>DONE</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>15</v>
@@ -1586,7 +1587,7 @@
       </c>
       <c r="C25" s="27" t="str">
         <f>C15</f>
-        <v>doplnit</v>
+        <v>DONE</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>15</v>

</xml_diff>